<commit_message>
Finished testing all, added archive function, created partstable class
</commit_message>
<xml_diff>
--- a/Test c#/Assets.xlsx
+++ b/Test c#/Assets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8760" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8760" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Senvion" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,17 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="2">
+  <si>
+    <t>Vendor ID</t>
+  </si>
+  <si>
+    <t>MPulse ID</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -352,34 +363,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,43 +424,85 @@
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>